<commit_message>
se agrego la hora de inicio de sesion
</commit_message>
<xml_diff>
--- a/pumpometer.xlsx
+++ b/pumpometer.xlsx
@@ -432,13 +432,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>328.8</v>
+        <v>325.7</v>
       </c>
       <c r="D2" t="n">
-        <v>328.9</v>
+        <v>325.9</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="3">
@@ -448,13 +448,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>328.7</v>
+        <v>325.3</v>
       </c>
       <c r="D3" t="n">
-        <v>328.6</v>
+        <v>325.7</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.03</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4">
@@ -528,13 +528,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>328.5</v>
+        <v>325.5</v>
       </c>
       <c r="D8" t="n">
-        <v>328.5</v>
+        <v>325.7</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
@@ -544,13 +544,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>29700</v>
+        <v>29517.89</v>
       </c>
       <c r="D9" t="n">
-        <v>29702.55</v>
+        <v>29512.68</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="10">
@@ -563,10 +563,10 @@
         <v>1.0011</v>
       </c>
       <c r="D10" t="n">
-        <v>1.0011</v>
+        <v>1.001</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="11">
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4069</v>
+        <v>0.4059</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4069</v>
+        <v>0.4057</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="12">
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1956.85</v>
+        <v>1941.02</v>
       </c>
       <c r="D12" t="n">
-        <v>1955.85</v>
+        <v>1940.71</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.05</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="13">
@@ -624,13 +624,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>68.40000000000001</v>
+        <v>68.2</v>
       </c>
       <c r="D14" t="n">
-        <v>68.5</v>
+        <v>68.2</v>
       </c>
       <c r="F14" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -640,13 +640,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>7.03</v>
+        <v>6.95</v>
       </c>
       <c r="D15" t="n">
-        <v>7.02</v>
+        <v>6.95</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -656,10 +656,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23.85</v>
+        <v>23.71</v>
       </c>
       <c r="D16" t="n">
-        <v>23.85</v>
+        <v>23.71</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -688,13 +688,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.08507000000000001</v>
+        <v>0.08466</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08519</v>
+        <v>0.08463</v>
       </c>
       <c r="F18" t="n">
-        <v>0.14</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="19">
@@ -704,13 +704,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.326</v>
+        <v>1.324</v>
       </c>
       <c r="D19" t="n">
-        <v>1.326</v>
+        <v>1.323</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="20">
@@ -720,13 +720,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1331</v>
+        <v>0.1322</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1332</v>
+        <v>0.1322</v>
       </c>
       <c r="F20" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -736,13 +736,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5162</v>
+        <v>0.514</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5163</v>
+        <v>0.514</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -752,13 +752,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>191.8</v>
+        <v>190.2</v>
       </c>
       <c r="D22" t="n">
-        <v>192.1</v>
+        <v>190.2</v>
       </c>
       <c r="F22" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>61.41</v>
+        <v>61.12</v>
       </c>
       <c r="D23" t="n">
-        <v>61.31</v>
+        <v>61.12</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -784,10 +784,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.094</v>
+        <v>4.06</v>
       </c>
       <c r="D24" t="n">
-        <v>4.094</v>
+        <v>4.06</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -800,13 +800,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.03169</v>
+        <v>0.03131</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03167</v>
+        <v>0.03131</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>16.411</v>
+        <v>16.448</v>
       </c>
       <c r="D26" t="n">
-        <v>16.414</v>
+        <v>16.45</v>
       </c>
       <c r="F26" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="27">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.069</v>
+        <v>1.068</v>
       </c>
       <c r="D27" t="n">
         <v>1.068</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.391</v>
+        <v>0.39</v>
       </c>
       <c r="D32" t="n">
         <v>0.39</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -944,10 +944,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.349</v>
+        <v>1.337</v>
       </c>
       <c r="D34" t="n">
-        <v>1.349</v>
+        <v>1.337</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -960,13 +960,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>10.79</v>
+        <v>10.73</v>
       </c>
       <c r="D35" t="n">
-        <v>10.78</v>
+        <v>10.73</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -976,13 +976,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>62.6</v>
+        <v>62.2</v>
       </c>
       <c r="D36" t="n">
-        <v>62.5</v>
+        <v>62.2</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -992,13 +992,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>11.77</v>
+        <v>11.65</v>
       </c>
       <c r="D37" t="n">
-        <v>11.74</v>
+        <v>11.65</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1008,10 +1008,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.49</v>
+        <v>5.47</v>
       </c>
       <c r="D38" t="n">
-        <v>5.49</v>
+        <v>5.47</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1024,13 +1024,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2.118</v>
+        <v>2.131</v>
       </c>
       <c r="D39" t="n">
-        <v>2.109</v>
+        <v>2.131</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1104,10 +1104,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.391</v>
+        <v>0.3895</v>
       </c>
       <c r="D44" t="n">
-        <v>0.391</v>
+        <v>0.3895</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1120,13 +1120,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1152,10 +1152,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2884</v>
+        <v>0.2872</v>
       </c>
       <c r="D47" t="n">
-        <v>0.2884</v>
+        <v>0.2872</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1168,10 +1168,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.02939</v>
+        <v>0.02919</v>
       </c>
       <c r="D48" t="n">
-        <v>0.02939</v>
+        <v>0.02919</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1216,13 +1216,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.4072</v>
+        <v>0.405</v>
       </c>
       <c r="D51" t="n">
-        <v>0.4072</v>
+        <v>0.4053</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="52">
@@ -1248,10 +1248,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.575</v>
+        <v>0.572</v>
       </c>
       <c r="D53" t="n">
-        <v>0.575</v>
+        <v>0.572</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1264,13 +1264,13 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>203.9</v>
+        <v>204.4</v>
       </c>
       <c r="D54" t="n">
-        <v>203.8</v>
+        <v>204.4</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1280,13 +1280,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>96.40000000000001</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="D55" t="n">
-        <v>96.09999999999999</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1344,10 +1344,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.03608</v>
+        <v>0.03578</v>
       </c>
       <c r="D59" t="n">
-        <v>0.03608</v>
+        <v>0.03578</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -1360,13 +1360,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>48.52</v>
+        <v>47.92</v>
       </c>
       <c r="D60" t="n">
-        <v>48.49</v>
+        <v>47.94</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.06</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="61">
@@ -1392,13 +1392,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.1888</v>
+        <v>0.1868</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1882</v>
+        <v>0.1872</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.32</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="63">
@@ -1424,10 +1424,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.0985</v>
+        <v>0.0975</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0985</v>
+        <v>0.0975</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -1440,13 +1440,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.652</v>
+        <v>0.646</v>
       </c>
       <c r="D65" t="n">
-        <v>0.65</v>
+        <v>0.645</v>
       </c>
       <c r="F65" t="n">
-        <v>-0.31</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="66">
@@ -1472,13 +1472,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.05171</v>
+        <v>0.05124</v>
       </c>
       <c r="D67" t="n">
-        <v>0.05185</v>
+        <v>0.05124</v>
       </c>
       <c r="F67" t="n">
-        <v>0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1488,13 +1488,13 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2.14</v>
+        <v>2.137</v>
       </c>
       <c r="D68" t="n">
-        <v>2.137</v>
+        <v>2.144</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.14</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="69">
@@ -1520,13 +1520,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.6159</v>
+        <v>0.6141</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6209</v>
+        <v>0.6139</v>
       </c>
       <c r="F70" t="n">
-        <v>0.8100000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="71">
@@ -1536,13 +1536,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.00621</v>
+        <v>0.00615</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00621</v>
+        <v>0.00618</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="72">
@@ -1568,10 +1568,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.01214</v>
+        <v>0.012</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01214</v>
+        <v>0.012</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -1584,10 +1584,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>66.40000000000001</v>
+        <v>65.7</v>
       </c>
       <c r="D74" t="n">
-        <v>66.40000000000001</v>
+        <v>65.7</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -1632,13 +1632,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.524</v>
+        <v>0.53</v>
       </c>
       <c r="D77" t="n">
-        <v>0.525</v>
+        <v>0.53</v>
       </c>
       <c r="F77" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1648,10 +1648,10 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2.574</v>
+        <v>2.549</v>
       </c>
       <c r="D78" t="n">
-        <v>2.574</v>
+        <v>2.549</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -1696,13 +1696,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.01217</v>
+        <v>0.01203</v>
       </c>
       <c r="D81" t="n">
-        <v>0.01215</v>
+        <v>0.01205</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="82">
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.5695</v>
+        <v>0.5642</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5695</v>
+        <v>0.5642</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -1744,10 +1744,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1273</v>
+        <v>1259</v>
       </c>
       <c r="D84" t="n">
-        <v>1273</v>
+        <v>1259</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -1776,13 +1776,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>3.131</v>
+        <v>3.087</v>
       </c>
       <c r="D86" t="n">
-        <v>3.124</v>
+        <v>3.087</v>
       </c>
       <c r="F86" t="n">
-        <v>-0.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1792,13 +1792,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>1.075</v>
+        <v>1.0554</v>
       </c>
       <c r="D87" t="n">
-        <v>1.0697</v>
+        <v>1.0551</v>
       </c>
       <c r="F87" t="n">
-        <v>-0.49</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="88">
@@ -1808,10 +1808,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.0833</v>
+        <v>0.0829</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0833</v>
+        <v>0.0829</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -1840,10 +1840,10 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.4201</v>
+        <v>0.4193</v>
       </c>
       <c r="D90" t="n">
-        <v>0.4201</v>
+        <v>0.4193</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -1856,13 +1856,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.7094</v>
+        <v>0.7092000000000001</v>
       </c>
       <c r="D91" t="n">
-        <v>0.7094</v>
+        <v>0.7091</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="92">
@@ -1872,10 +1872,10 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.0541</v>
+        <v>0.0537</v>
       </c>
       <c r="D92" t="n">
-        <v>0.0541</v>
+        <v>0.0537</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -1888,10 +1888,10 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.717</v>
+        <v>0.716</v>
       </c>
       <c r="D93" t="n">
-        <v>0.717</v>
+        <v>0.716</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -1920,13 +1920,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.3406</v>
+        <v>0.3342</v>
       </c>
       <c r="D95" t="n">
-        <v>0.3377</v>
+        <v>0.3342</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -1936,10 +1936,10 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>7.55</v>
+        <v>7.49</v>
       </c>
       <c r="D96" t="n">
-        <v>7.55</v>
+        <v>7.49</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -1952,13 +1952,13 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>8575.889999999999</v>
+        <v>8463.629999999999</v>
       </c>
       <c r="D97" t="n">
-        <v>8569</v>
+        <v>8463.629999999999</v>
       </c>
       <c r="F97" t="n">
-        <v>-0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2000,13 +2000,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>1.0001</v>
+        <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>1.0002</v>
+        <v>1</v>
       </c>
       <c r="F100" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2016,13 +2016,13 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.04441</v>
+        <v>0.04414</v>
       </c>
       <c r="D101" t="n">
-        <v>0.04441</v>
+        <v>0.04423</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="102">
@@ -2032,10 +2032,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>1.131</v>
+        <v>1.127</v>
       </c>
       <c r="D102" t="n">
-        <v>1.131</v>
+        <v>1.127</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -2048,10 +2048,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1.869</v>
+        <v>1.839</v>
       </c>
       <c r="D103" t="n">
-        <v>1.869</v>
+        <v>1.839</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>1.254</v>
+        <v>1.234</v>
       </c>
       <c r="D104" t="n">
-        <v>1.254</v>
+        <v>1.234</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -2080,13 +2080,13 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>1.4158</v>
+        <v>1.3854</v>
       </c>
       <c r="D105" t="n">
-        <v>1.4086</v>
+        <v>1.3867</v>
       </c>
       <c r="F105" t="n">
-        <v>-0.51</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="106">
@@ -2096,13 +2096,13 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.2277</v>
+        <v>0.224</v>
       </c>
       <c r="D106" t="n">
-        <v>0.2266</v>
+        <v>0.224</v>
       </c>
       <c r="F106" t="n">
-        <v>-0.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2112,10 +2112,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>12.51</v>
+        <v>12.53</v>
       </c>
       <c r="D107" t="n">
-        <v>12.51</v>
+        <v>12.53</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -2128,13 +2128,13 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>9.970000000000001</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="D108" t="n">
-        <v>9.949999999999999</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="F108" t="n">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2144,13 +2144,13 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.0001868</v>
+        <v>0.0001808</v>
       </c>
       <c r="D109" t="n">
-        <v>0.0001858</v>
+        <v>0.00018087</v>
       </c>
       <c r="F109" t="n">
-        <v>-0.54</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="110">
@@ -2160,13 +2160,13 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.08069</v>
+        <v>0.08018</v>
       </c>
       <c r="D110" t="n">
-        <v>0.08081000000000001</v>
+        <v>0.08018</v>
       </c>
       <c r="F110" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -2176,13 +2176,13 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.00587</v>
+        <v>0.00583</v>
       </c>
       <c r="D111" t="n">
-        <v>0.0059</v>
+        <v>0.00583</v>
       </c>
       <c r="F111" t="n">
-        <v>0.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -2192,10 +2192,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>1859</v>
+        <v>1855</v>
       </c>
       <c r="D112" t="n">
-        <v>1859</v>
+        <v>1855</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
@@ -2224,10 +2224,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>9.529999999999999</v>
+        <v>9.43</v>
       </c>
       <c r="D114" t="n">
-        <v>9.529999999999999</v>
+        <v>9.43</v>
       </c>
       <c r="F114" t="n">
         <v>0</v>
@@ -2240,13 +2240,13 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>9.57</v>
+        <v>9.44</v>
       </c>
       <c r="D115" t="n">
-        <v>9.550000000000001</v>
+        <v>9.44</v>
       </c>
       <c r="F115" t="n">
-        <v>-0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -2272,10 +2272,10 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>1.669</v>
+        <v>1.652</v>
       </c>
       <c r="D117" t="n">
-        <v>1.669</v>
+        <v>1.652</v>
       </c>
       <c r="F117" t="n">
         <v>0</v>
@@ -2304,10 +2304,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>80.40000000000001</v>
+        <v>79.2</v>
       </c>
       <c r="D119" t="n">
-        <v>80.40000000000001</v>
+        <v>79.2</v>
       </c>
       <c r="F119" t="n">
         <v>0</v>
@@ -2320,13 +2320,13 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>87.77</v>
+        <v>87.33</v>
       </c>
       <c r="D120" t="n">
-        <v>87.81999999999999</v>
+        <v>87.33</v>
       </c>
       <c r="F120" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -2336,10 +2336,10 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.461</v>
+        <v>0.455</v>
       </c>
       <c r="D121" t="n">
-        <v>0.461</v>
+        <v>0.455</v>
       </c>
       <c r="F121" t="n">
         <v>0</v>
@@ -2352,10 +2352,10 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.4</v>
+        <v>0.395</v>
       </c>
       <c r="D122" t="n">
-        <v>0.401</v>
+        <v>0.396</v>
       </c>
       <c r="F122" t="n">
         <v>0.25</v>
@@ -2384,10 +2384,10 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>3.72</v>
+        <v>3.66</v>
       </c>
       <c r="D124" t="n">
-        <v>3.72</v>
+        <v>3.66</v>
       </c>
       <c r="F124" t="n">
         <v>0</v>
@@ -2400,13 +2400,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>24.3</v>
+        <v>24.8</v>
       </c>
       <c r="D125" t="n">
-        <v>24.4</v>
+        <v>24.8</v>
       </c>
       <c r="F125" t="n">
-        <v>0.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -2416,10 +2416,10 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>5.64</v>
+        <v>5.61</v>
       </c>
       <c r="D126" t="n">
-        <v>5.64</v>
+        <v>5.61</v>
       </c>
       <c r="F126" t="n">
         <v>0</v>
@@ -2432,13 +2432,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>27.53</v>
+        <v>27.21</v>
       </c>
       <c r="D127" t="n">
-        <v>27.52</v>
+        <v>27.23</v>
       </c>
       <c r="F127" t="n">
-        <v>-0.04</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="128">
@@ -2464,13 +2464,13 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>4.811</v>
+        <v>4.772</v>
       </c>
       <c r="D129" t="n">
-        <v>4.809</v>
+        <v>4.777</v>
       </c>
       <c r="F129" t="n">
-        <v>-0.04</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="130">
@@ -2480,13 +2480,13 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>4.61</v>
+        <v>4.59</v>
       </c>
       <c r="D130" t="n">
-        <v>4.61</v>
+        <v>4.58</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="131">
@@ -2496,13 +2496,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.1661</v>
+        <v>0.1649</v>
       </c>
       <c r="D131" t="n">
-        <v>0.1662</v>
+        <v>0.1649</v>
       </c>
       <c r="F131" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -2512,10 +2512,10 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.2077</v>
+        <v>0.2037</v>
       </c>
       <c r="D132" t="n">
-        <v>0.2077</v>
+        <v>0.2037</v>
       </c>
       <c r="F132" t="n">
         <v>0</v>
@@ -2528,13 +2528,13 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>103.7</v>
+        <v>102</v>
       </c>
       <c r="D133" t="n">
-        <v>103.5</v>
+        <v>102</v>
       </c>
       <c r="F133" t="n">
-        <v>-0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -2544,13 +2544,13 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>5.767</v>
+        <v>5.753</v>
       </c>
       <c r="D134" t="n">
-        <v>5.757</v>
+        <v>5.753</v>
       </c>
       <c r="F134" t="n">
-        <v>-0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -2560,10 +2560,10 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>8.24</v>
+        <v>8.17</v>
       </c>
       <c r="D135" t="n">
-        <v>8.24</v>
+        <v>8.17</v>
       </c>
       <c r="F135" t="n">
         <v>0</v>
@@ -2576,13 +2576,13 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>2.247</v>
+        <v>2.225</v>
       </c>
       <c r="D136" t="n">
-        <v>2.247</v>
+        <v>2.227</v>
       </c>
       <c r="F136" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="137">
@@ -2592,10 +2592,10 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.1463</v>
+        <v>0.1471</v>
       </c>
       <c r="D137" t="n">
-        <v>0.1463</v>
+        <v>0.1471</v>
       </c>
       <c r="F137" t="n">
         <v>0</v>
@@ -2608,13 +2608,13 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.04679</v>
+        <v>0.04618</v>
       </c>
       <c r="D138" t="n">
-        <v>0.04664</v>
+        <v>0.04618</v>
       </c>
       <c r="F138" t="n">
-        <v>-0.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -2624,13 +2624,13 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.486</v>
+        <v>0.477</v>
       </c>
       <c r="D139" t="n">
-        <v>0.487</v>
+        <v>0.477</v>
       </c>
       <c r="F139" t="n">
-        <v>0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -2640,10 +2640,10 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.803</v>
+        <v>0.793</v>
       </c>
       <c r="D140" t="n">
-        <v>0.803</v>
+        <v>0.793</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
@@ -2672,13 +2672,13 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>143.86</v>
+        <v>142.9</v>
       </c>
       <c r="D142" t="n">
-        <v>143.73</v>
+        <v>142.73</v>
       </c>
       <c r="F142" t="n">
-        <v>-0.09</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="143">
@@ -2688,13 +2688,13 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>21.14</v>
+        <v>20.85</v>
       </c>
       <c r="D143" t="n">
-        <v>21.11</v>
+        <v>20.85</v>
       </c>
       <c r="F143" t="n">
-        <v>-0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -2704,10 +2704,10 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.2435</v>
+        <v>0.2424</v>
       </c>
       <c r="D144" t="n">
-        <v>0.2435</v>
+        <v>0.2424</v>
       </c>
       <c r="F144" t="n">
         <v>0</v>
@@ -2720,10 +2720,10 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.053</v>
+        <v>0.0528</v>
       </c>
       <c r="D145" t="n">
-        <v>0.053</v>
+        <v>0.0528</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -2736,10 +2736,10 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.351</v>
+        <v>0.346</v>
       </c>
       <c r="D146" t="n">
-        <v>0.351</v>
+        <v>0.346</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
@@ -2752,10 +2752,10 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.582</v>
+        <v>0.583</v>
       </c>
       <c r="D147" t="n">
-        <v>0.582</v>
+        <v>0.583</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>
@@ -2768,13 +2768,13 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.01997</v>
+        <v>0.02053</v>
       </c>
       <c r="D148" t="n">
-        <v>0.01982</v>
+        <v>0.02048</v>
       </c>
       <c r="F148" t="n">
-        <v>-0.75</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="149">
@@ -2784,13 +2784,13 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>2.401</v>
+        <v>2.379</v>
       </c>
       <c r="D149" t="n">
-        <v>2.398</v>
+        <v>2.379</v>
       </c>
       <c r="F149" t="n">
-        <v>-0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -2800,13 +2800,13 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.2687</v>
+        <v>0.2672</v>
       </c>
       <c r="D150" t="n">
-        <v>0.2697</v>
+        <v>0.2672</v>
       </c>
       <c r="F150" t="n">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -2832,13 +2832,13 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.07019</v>
+        <v>0.06938999999999999</v>
       </c>
       <c r="D152" t="n">
-        <v>0.06998</v>
+        <v>0.06937</v>
       </c>
       <c r="F152" t="n">
-        <v>-0.3</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="153">
@@ -2848,13 +2848,13 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>4.859</v>
+        <v>4.854</v>
       </c>
       <c r="D153" t="n">
-        <v>4.86</v>
+        <v>4.853</v>
       </c>
       <c r="F153" t="n">
-        <v>0.02</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="154">
@@ -2864,13 +2864,13 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.1968</v>
+        <v>0.1941</v>
       </c>
       <c r="D154" t="n">
-        <v>0.1968</v>
+        <v>0.1944</v>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="155">
@@ -2896,10 +2896,10 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>4.66</v>
+        <v>4.67</v>
       </c>
       <c r="D156" t="n">
-        <v>4.66</v>
+        <v>4.67</v>
       </c>
       <c r="F156" t="n">
         <v>0</v>
@@ -2912,10 +2912,10 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.0842</v>
+        <v>0.0828</v>
       </c>
       <c r="D157" t="n">
-        <v>0.0842</v>
+        <v>0.0828</v>
       </c>
       <c r="F157" t="n">
         <v>0</v>
@@ -2944,10 +2944,10 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>1.548</v>
+        <v>1.544</v>
       </c>
       <c r="D159" t="n">
-        <v>1.548</v>
+        <v>1.544</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>
@@ -2976,13 +2976,13 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>4.11</v>
+        <v>4.05</v>
       </c>
       <c r="D161" t="n">
-        <v>4.12</v>
+        <v>4.07</v>
       </c>
       <c r="F161" t="n">
-        <v>0.24</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="162">
@@ -2992,13 +2992,13 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>8.140000000000001</v>
+        <v>8.15</v>
       </c>
       <c r="D162" t="n">
-        <v>8.119999999999999</v>
+        <v>8.15</v>
       </c>
       <c r="F162" t="n">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -3024,10 +3024,10 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>8.210000000000001</v>
+        <v>8.17</v>
       </c>
       <c r="D164" t="n">
-        <v>8.210000000000001</v>
+        <v>8.17</v>
       </c>
       <c r="F164" t="n">
         <v>0</v>
@@ -3056,10 +3056,10 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>3.32</v>
+        <v>3.3</v>
       </c>
       <c r="D166" t="n">
-        <v>3.32</v>
+        <v>3.3</v>
       </c>
       <c r="F166" t="n">
         <v>0</v>
@@ -3072,13 +3072,13 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>1</v>
+        <v>1.0001</v>
       </c>
       <c r="D167" t="n">
         <v>1.0001</v>
       </c>
       <c r="F167" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -3088,13 +3088,13 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.9999</v>
+        <v>1</v>
       </c>
       <c r="D168" t="n">
         <v>1</v>
       </c>
       <c r="F168" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -3120,10 +3120,10 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.00478</v>
+        <v>0.00474</v>
       </c>
       <c r="D170" t="n">
-        <v>0.00478</v>
+        <v>0.00474</v>
       </c>
       <c r="F170" t="n">
         <v>0</v>
@@ -3136,10 +3136,10 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.00477</v>
+        <v>0.00473</v>
       </c>
       <c r="D171" t="n">
-        <v>0.00477</v>
+        <v>0.00473</v>
       </c>
       <c r="F171" t="n">
         <v>0</v>
@@ -3152,10 +3152,10 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.6551</v>
+        <v>0.648</v>
       </c>
       <c r="D172" t="n">
-        <v>0.6551</v>
+        <v>0.648</v>
       </c>
       <c r="F172" t="n">
         <v>0</v>
@@ -3168,13 +3168,13 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.674</v>
+        <v>0.665</v>
       </c>
       <c r="D173" t="n">
-        <v>0.673</v>
+        <v>0.666</v>
       </c>
       <c r="F173" t="n">
-        <v>-0.15</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="174">
@@ -3200,10 +3200,10 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.4243</v>
+        <v>0.4168</v>
       </c>
       <c r="D175" t="n">
-        <v>0.4243</v>
+        <v>0.4168</v>
       </c>
       <c r="F175" t="n">
         <v>0</v>
@@ -3216,13 +3216,13 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>7.396</v>
+        <v>7.315</v>
       </c>
       <c r="D176" t="n">
-        <v>7.499</v>
+        <v>7.304</v>
       </c>
       <c r="F176" t="n">
-        <v>1.39</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="177">
@@ -3248,13 +3248,13 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.336</v>
+        <v>0.331</v>
       </c>
       <c r="D178" t="n">
-        <v>0.334</v>
+        <v>0.331</v>
       </c>
       <c r="F178" t="n">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -3264,13 +3264,13 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.2244</v>
+        <v>0.2174</v>
       </c>
       <c r="D179" t="n">
-        <v>0.2239</v>
+        <v>0.2174</v>
       </c>
       <c r="F179" t="n">
-        <v>-0.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -3280,10 +3280,10 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.973</v>
+        <v>0.966</v>
       </c>
       <c r="D180" t="n">
-        <v>0.973</v>
+        <v>0.966</v>
       </c>
       <c r="F180" t="n">
         <v>0</v>
@@ -3296,10 +3296,10 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>1.711</v>
+        <v>1.686</v>
       </c>
       <c r="D181" t="n">
-        <v>1.711</v>
+        <v>1.686</v>
       </c>
       <c r="F181" t="n">
         <v>0</v>
@@ -3312,10 +3312,10 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="D182" t="n">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="F182" t="n">
         <v>0</v>
@@ -3328,13 +3328,13 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.01723</v>
+        <v>0.01717</v>
       </c>
       <c r="D183" t="n">
-        <v>0.01721</v>
+        <v>0.01717</v>
       </c>
       <c r="F183" t="n">
-        <v>-0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>2.54</v>
+        <v>2.536</v>
       </c>
       <c r="D184" t="n">
-        <v>2.54</v>
+        <v>2.536</v>
       </c>
       <c r="F184" t="n">
         <v>0</v>
@@ -3360,13 +3360,13 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.00432</v>
+        <v>0.00428</v>
       </c>
       <c r="D185" t="n">
-        <v>0.00431</v>
+        <v>0.00428</v>
       </c>
       <c r="F185" t="n">
-        <v>-0.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -3376,13 +3376,13 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>3.869</v>
+        <v>3.79</v>
       </c>
       <c r="D186" t="n">
-        <v>3.875</v>
+        <v>3.79</v>
       </c>
       <c r="F186" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -3392,10 +3392,10 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>6.44</v>
+        <v>6.37</v>
       </c>
       <c r="D187" t="n">
-        <v>6.44</v>
+        <v>6.37</v>
       </c>
       <c r="F187" t="n">
         <v>0</v>
@@ -3424,10 +3424,10 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.0424</v>
+        <v>0.0421</v>
       </c>
       <c r="D189" t="n">
-        <v>0.0424</v>
+        <v>0.0421</v>
       </c>
       <c r="F189" t="n">
         <v>0</v>
@@ -3440,13 +3440,13 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>6.02</v>
+        <v>5.98</v>
       </c>
       <c r="D190" t="n">
-        <v>6.01</v>
+        <v>5.98</v>
       </c>
       <c r="F190" t="n">
-        <v>-0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -3456,13 +3456,13 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.3639</v>
+        <v>0.3563</v>
       </c>
       <c r="D191" t="n">
-        <v>0.3609</v>
+        <v>0.3567</v>
       </c>
       <c r="F191" t="n">
-        <v>-0.82</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="192">
@@ -3472,10 +3472,10 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.053</v>
+        <v>0.0527</v>
       </c>
       <c r="D192" t="n">
-        <v>0.053</v>
+        <v>0.0527</v>
       </c>
       <c r="F192" t="n">
         <v>0</v>
@@ -3488,10 +3488,10 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.01125</v>
+        <v>0.01101</v>
       </c>
       <c r="D193" t="n">
-        <v>0.01125</v>
+        <v>0.01101</v>
       </c>
       <c r="F193" t="n">
         <v>0</v>
@@ -3504,10 +3504,10 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="D194" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="F194" t="n">
         <v>0</v>
@@ -3520,13 +3520,13 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>2.9</v>
+        <v>2.85</v>
       </c>
       <c r="D195" t="n">
-        <v>2.89</v>
+        <v>2.85</v>
       </c>
       <c r="F195" t="n">
-        <v>-0.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -3536,10 +3536,10 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.1204</v>
+        <v>0.12</v>
       </c>
       <c r="D196" t="n">
-        <v>0.1204</v>
+        <v>0.12</v>
       </c>
       <c r="F196" t="n">
         <v>0</v>
@@ -3552,13 +3552,13 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>672.2</v>
+        <v>662</v>
       </c>
       <c r="D197" t="n">
-        <v>672.2</v>
+        <v>662.4</v>
       </c>
       <c r="F197" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="198">
@@ -3568,13 +3568,13 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.00997</v>
+        <v>0.009730000000000001</v>
       </c>
       <c r="D198" t="n">
-        <v>0.009979999999999999</v>
+        <v>0.009730000000000001</v>
       </c>
       <c r="F198" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -3584,10 +3584,10 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>1.32</v>
+        <v>1.29</v>
       </c>
       <c r="D199" t="n">
-        <v>1.32</v>
+        <v>1.29</v>
       </c>
       <c r="F199" t="n">
         <v>0</v>
@@ -3600,10 +3600,10 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.0407</v>
+        <v>0.0402</v>
       </c>
       <c r="D200" t="n">
-        <v>0.0407</v>
+        <v>0.0402</v>
       </c>
       <c r="F200" t="n">
         <v>0</v>
@@ -3616,10 +3616,10 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.2151</v>
+        <v>0.2113</v>
       </c>
       <c r="D201" t="n">
-        <v>0.2151</v>
+        <v>0.2113</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
@@ -3632,10 +3632,10 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.0886</v>
+        <v>0.0882</v>
       </c>
       <c r="D202" t="n">
-        <v>0.0886</v>
+        <v>0.0882</v>
       </c>
       <c r="F202" t="n">
         <v>0</v>
@@ -3648,10 +3648,10 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.00512</v>
+        <v>0.00507</v>
       </c>
       <c r="D203" t="n">
-        <v>0.00512</v>
+        <v>0.00507</v>
       </c>
       <c r="F203" t="n">
         <v>0</v>
@@ -3680,13 +3680,13 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>174.5</v>
+        <v>174.4</v>
       </c>
       <c r="D205" t="n">
-        <v>175.2</v>
+        <v>174.4</v>
       </c>
       <c r="F205" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206">
@@ -3696,10 +3696,10 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.399</v>
+        <v>0.393</v>
       </c>
       <c r="D206" t="n">
-        <v>0.399</v>
+        <v>0.393</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
@@ -3712,10 +3712,10 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.0364</v>
+        <v>0.0359</v>
       </c>
       <c r="D207" t="n">
-        <v>0.0364</v>
+        <v>0.0359</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
@@ -3728,13 +3728,13 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>23.35</v>
+        <v>23.18</v>
       </c>
       <c r="D208" t="n">
-        <v>23.1</v>
+        <v>23.25</v>
       </c>
       <c r="F208" t="n">
-        <v>-1.07</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="209">
@@ -3744,13 +3744,13 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.002548</v>
+        <v>0.002512</v>
       </c>
       <c r="D209" t="n">
-        <v>0.002543</v>
+        <v>0.002512</v>
       </c>
       <c r="F209" t="n">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -3760,13 +3760,13 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.36898</v>
+        <v>0.35967</v>
       </c>
       <c r="D210" t="n">
-        <v>0.36863</v>
+        <v>0.35984</v>
       </c>
       <c r="F210" t="n">
-        <v>-0.09</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="211">
@@ -3776,13 +3776,13 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="D211" t="n">
-        <v>4.67</v>
+        <v>4.65</v>
       </c>
       <c r="F211" t="n">
-        <v>-0.64</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="212">
@@ -3792,10 +3792,10 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>3.38</v>
+        <v>3.4</v>
       </c>
       <c r="D212" t="n">
-        <v>3.38</v>
+        <v>3.4</v>
       </c>
       <c r="F212" t="n">
         <v>0</v>
@@ -3808,13 +3808,13 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.929</v>
+        <v>0.955</v>
       </c>
       <c r="D213" t="n">
-        <v>0.93</v>
+        <v>0.949</v>
       </c>
       <c r="F213" t="n">
-        <v>0.11</v>
+        <v>-0.63</v>
       </c>
     </row>
     <row r="214">
@@ -3824,13 +3824,13 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.00564</v>
+        <v>0.00557</v>
       </c>
       <c r="D214" t="n">
-        <v>0.00564</v>
+        <v>0.00555</v>
       </c>
       <c r="F214" t="n">
-        <v>0</v>
+        <v>-0.36</v>
       </c>
     </row>
     <row r="215">
@@ -3840,10 +3840,10 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>1.164e-05</v>
+        <v>1.16e-05</v>
       </c>
       <c r="D215" t="n">
-        <v>1.165e-05</v>
+        <v>1.161e-05</v>
       </c>
       <c r="F215" t="n">
         <v>0.09</v>
@@ -3856,13 +3856,13 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>1.163e-05</v>
+        <v>1.16e-05</v>
       </c>
       <c r="D216" t="n">
-        <v>1.164e-05</v>
+        <v>1.16e-05</v>
       </c>
       <c r="F216" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -3872,10 +3872,10 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>7.87</v>
+        <v>7.79</v>
       </c>
       <c r="D217" t="n">
-        <v>7.87</v>
+        <v>7.79</v>
       </c>
       <c r="F217" t="n">
         <v>0</v>
@@ -3888,10 +3888,10 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>14.7</v>
+        <v>14.53</v>
       </c>
       <c r="D218" t="n">
-        <v>14.7</v>
+        <v>14.53</v>
       </c>
       <c r="F218" t="n">
         <v>0</v>
@@ -3904,13 +3904,13 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.646</v>
+        <v>0.64</v>
       </c>
       <c r="D219" t="n">
-        <v>0.648</v>
+        <v>0.64</v>
       </c>
       <c r="F219" t="n">
-        <v>0.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -3920,13 +3920,13 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.1071</v>
+        <v>0.1064</v>
       </c>
       <c r="D220" t="n">
-        <v>0.1071</v>
+        <v>0.1062</v>
       </c>
       <c r="F220" t="n">
-        <v>0</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="221">
@@ -3936,13 +3936,13 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>1.927</v>
+        <v>1.913</v>
       </c>
       <c r="D221" t="n">
-        <v>1.923</v>
+        <v>1.913</v>
       </c>
       <c r="F221" t="n">
-        <v>-0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -3952,10 +3952,10 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>13.34</v>
+        <v>13.27</v>
       </c>
       <c r="D222" t="n">
-        <v>13.34</v>
+        <v>13.27</v>
       </c>
       <c r="F222" t="n">
         <v>0</v>
@@ -4000,13 +4000,13 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.01822</v>
+        <v>0.01806</v>
       </c>
       <c r="D225" t="n">
-        <v>0.01822</v>
+        <v>0.01807</v>
       </c>
       <c r="F225" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="226">
@@ -4016,13 +4016,13 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>4.31</v>
+        <v>4.36</v>
       </c>
       <c r="D226" t="n">
-        <v>4.42</v>
+        <v>4.35</v>
       </c>
       <c r="F226" t="n">
-        <v>2.55</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="227">
@@ -4032,10 +4032,10 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>20.51</v>
+        <v>20.33</v>
       </c>
       <c r="D227" t="n">
-        <v>20.51</v>
+        <v>20.33</v>
       </c>
       <c r="F227" t="n">
         <v>0</v>
@@ -4048,13 +4048,13 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.4079</v>
+        <v>0.4027</v>
       </c>
       <c r="D228" t="n">
-        <v>0.4082</v>
+        <v>0.4025</v>
       </c>
       <c r="F228" t="n">
-        <v>0.07000000000000001</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="229">
@@ -4064,10 +4064,10 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>1.244</v>
+        <v>1.23</v>
       </c>
       <c r="D229" t="n">
-        <v>1.244</v>
+        <v>1.23</v>
       </c>
       <c r="F229" t="n">
         <v>0</v>
@@ -4080,13 +4080,13 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.0001657</v>
+        <v>0.000164</v>
       </c>
       <c r="D230" t="n">
-        <v>0.0001651</v>
+        <v>0.000164</v>
       </c>
       <c r="F230" t="n">
-        <v>-0.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -4096,10 +4096,10 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>2.72</v>
+        <v>2.697</v>
       </c>
       <c r="D231" t="n">
-        <v>2.72</v>
+        <v>2.697</v>
       </c>
       <c r="F231" t="n">
         <v>0</v>
@@ -4128,13 +4128,13 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.1648</v>
+        <v>0.1635</v>
       </c>
       <c r="D233" t="n">
-        <v>0.1649</v>
+        <v>0.1635</v>
       </c>
       <c r="F233" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -4144,10 +4144,10 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>2.649</v>
+        <v>2.621</v>
       </c>
       <c r="D234" t="n">
-        <v>2.649</v>
+        <v>2.621</v>
       </c>
       <c r="F234" t="n">
         <v>0</v>
@@ -4160,10 +4160,10 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>30.7</v>
+        <v>30.33</v>
       </c>
       <c r="D235" t="n">
-        <v>30.7</v>
+        <v>30.33</v>
       </c>
       <c r="F235" t="n">
         <v>0</v>
@@ -4176,13 +4176,13 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.1213</v>
+        <v>0.1202</v>
       </c>
       <c r="D236" t="n">
-        <v>0.121</v>
+        <v>0.1202</v>
       </c>
       <c r="F236" t="n">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -4208,13 +4208,13 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.00539</v>
+        <v>0.00534</v>
       </c>
       <c r="D238" t="n">
-        <v>0.00539</v>
+        <v>0.00537</v>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="239">
@@ -4224,13 +4224,13 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.2162</v>
+        <v>0.2142</v>
       </c>
       <c r="D239" t="n">
-        <v>0.2158</v>
+        <v>0.2142</v>
       </c>
       <c r="F239" t="n">
-        <v>-0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -4240,13 +4240,13 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.01017</v>
+        <v>0.01009</v>
       </c>
       <c r="D240" t="n">
-        <v>0.01016</v>
+        <v>0.01009</v>
       </c>
       <c r="F240" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -4256,10 +4256,10 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>7.56</v>
+        <v>7.52</v>
       </c>
       <c r="D241" t="n">
-        <v>7.56</v>
+        <v>7.52</v>
       </c>
       <c r="F241" t="n">
         <v>0</v>
@@ -4272,13 +4272,13 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>29.17</v>
+        <v>28.97</v>
       </c>
       <c r="D242" t="n">
-        <v>29.17</v>
+        <v>28.98</v>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="243">
@@ -4288,10 +4288,10 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.02234</v>
+        <v>0.02193</v>
       </c>
       <c r="D243" t="n">
-        <v>0.02234</v>
+        <v>0.02193</v>
       </c>
       <c r="F243" t="n">
         <v>0</v>
@@ -4304,10 +4304,10 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>2.14</v>
+        <v>2.097</v>
       </c>
       <c r="D244" t="n">
-        <v>2.14</v>
+        <v>2.097</v>
       </c>
       <c r="F244" t="n">
         <v>0</v>
@@ -4320,13 +4320,13 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.467</v>
+        <v>0.463</v>
       </c>
       <c r="D245" t="n">
-        <v>0.467</v>
+        <v>0.462</v>
       </c>
       <c r="F245" t="n">
-        <v>0</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="246">
@@ -4336,10 +4336,10 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.1537</v>
+        <v>0.1531</v>
       </c>
       <c r="D246" t="n">
-        <v>0.1537</v>
+        <v>0.1531</v>
       </c>
       <c r="F246" t="n">
         <v>0</v>
@@ -4352,10 +4352,10 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.0403</v>
+        <v>0.03951</v>
       </c>
       <c r="D247" t="n">
-        <v>0.0403</v>
+        <v>0.03951</v>
       </c>
       <c r="F247" t="n">
         <v>0</v>
@@ -4368,13 +4368,13 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>35.46</v>
+        <v>35.5</v>
       </c>
       <c r="D248" t="n">
-        <v>35.45</v>
+        <v>35.5</v>
       </c>
       <c r="F248" t="n">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -4384,10 +4384,10 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>3.66</v>
+        <v>3.58</v>
       </c>
       <c r="D249" t="n">
-        <v>3.66</v>
+        <v>3.58</v>
       </c>
       <c r="F249" t="n">
         <v>0</v>
@@ -4400,10 +4400,10 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>29.2</v>
+        <v>29</v>
       </c>
       <c r="D250" t="n">
-        <v>29.2</v>
+        <v>29</v>
       </c>
       <c r="F250" t="n">
         <v>0</v>
@@ -4416,13 +4416,13 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>0.0985</v>
+        <v>0.0979</v>
       </c>
       <c r="D251" t="n">
-        <v>0.0984</v>
+        <v>0.0979</v>
       </c>
       <c r="F251" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252">
@@ -4432,10 +4432,10 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>0.2329</v>
+        <v>0.2316</v>
       </c>
       <c r="D252" t="n">
-        <v>0.2329</v>
+        <v>0.2316</v>
       </c>
       <c r="F252" t="n">
         <v>0</v>
@@ -4448,10 +4448,10 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>78.8</v>
+        <v>77.7</v>
       </c>
       <c r="D253" t="n">
-        <v>78.8</v>
+        <v>77.7</v>
       </c>
       <c r="F253" t="n">
         <v>0</v>
@@ -4467,10 +4467,10 @@
         <v>0.659</v>
       </c>
       <c r="D254" t="n">
-        <v>0.661</v>
+        <v>0.659</v>
       </c>
       <c r="F254" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255">
@@ -4480,13 +4480,13 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.147</v>
+        <v>0.146</v>
       </c>
       <c r="D255" t="n">
         <v>0.147</v>
       </c>
       <c r="F255" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="256">
@@ -4496,10 +4496,10 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>67.40000000000001</v>
+        <v>67</v>
       </c>
       <c r="D256" t="n">
-        <v>67.40000000000001</v>
+        <v>67</v>
       </c>
       <c r="F256" t="n">
         <v>0</v>
@@ -4512,10 +4512,10 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>2.7</v>
+        <v>2.68</v>
       </c>
       <c r="D257" t="n">
-        <v>2.7</v>
+        <v>2.68</v>
       </c>
       <c r="F257" t="n">
         <v>0</v>
@@ -4528,13 +4528,13 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>4.941e-05</v>
+        <v>4.915e-05</v>
       </c>
       <c r="D258" t="n">
-        <v>4.945e-05</v>
+        <v>4.915e-05</v>
       </c>
       <c r="F258" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -4544,13 +4544,13 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.988</v>
+        <v>0.977</v>
       </c>
       <c r="D259" t="n">
-        <v>0.986</v>
+        <v>0.977</v>
       </c>
       <c r="F259" t="n">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -4560,10 +4560,10 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.992</v>
+        <v>0.979</v>
       </c>
       <c r="D260" t="n">
-        <v>0.992</v>
+        <v>0.979</v>
       </c>
       <c r="F260" t="n">
         <v>0</v>
@@ -4576,10 +4576,10 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>49.7</v>
+        <v>49.3</v>
       </c>
       <c r="D261" t="n">
-        <v>49.7</v>
+        <v>49.3</v>
       </c>
       <c r="F261" t="n">
         <v>0</v>
@@ -4595,10 +4595,10 @@
         <v>0.3161</v>
       </c>
       <c r="D262" t="n">
-        <v>0.3163</v>
+        <v>0.3161</v>
       </c>
       <c r="F262" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -4608,10 +4608,10 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>1.499</v>
+        <v>1.489</v>
       </c>
       <c r="D263" t="n">
-        <v>1.499</v>
+        <v>1.489</v>
       </c>
       <c r="F263" t="n">
         <v>0</v>
@@ -4624,13 +4624,13 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.998</v>
+        <v>0.988</v>
       </c>
       <c r="D264" t="n">
-        <v>0.999</v>
+        <v>0.988</v>
       </c>
       <c r="F264" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -4640,13 +4640,13 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>0.1282</v>
+        <v>0.1284</v>
       </c>
       <c r="D265" t="n">
-        <v>0.1288</v>
+        <v>0.1284</v>
       </c>
       <c r="F265" t="n">
-        <v>0.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -4656,10 +4656,10 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.2504</v>
+        <v>0.2486</v>
       </c>
       <c r="D266" t="n">
-        <v>0.2504</v>
+        <v>0.2486</v>
       </c>
       <c r="F266" t="n">
         <v>0</v>
@@ -4688,10 +4688,10 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>1.382</v>
+        <v>1.39</v>
       </c>
       <c r="D268" t="n">
-        <v>1.382</v>
+        <v>1.39</v>
       </c>
       <c r="F268" t="n">
         <v>0</v>
@@ -4704,10 +4704,10 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.2262</v>
+        <v>0.222</v>
       </c>
       <c r="D269" t="n">
-        <v>0.2262</v>
+        <v>0.222</v>
       </c>
       <c r="F269" t="n">
         <v>0</v>
@@ -4720,10 +4720,10 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.243</v>
+        <v>0.2412</v>
       </c>
       <c r="D270" t="n">
-        <v>0.243</v>
+        <v>0.2412</v>
       </c>
       <c r="F270" t="n">
         <v>0</v>
@@ -4736,13 +4736,13 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>2.098</v>
+        <v>2.078</v>
       </c>
       <c r="D271" t="n">
-        <v>2.097</v>
+        <v>2.076</v>
       </c>
       <c r="F271" t="n">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="272">
@@ -4752,13 +4752,13 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.1613</v>
+        <v>0.1599</v>
       </c>
       <c r="D272" t="n">
-        <v>0.1616</v>
+        <v>0.1599</v>
       </c>
       <c r="F272" t="n">
-        <v>0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -4784,10 +4784,10 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>1</v>
+        <v>1.0001</v>
       </c>
       <c r="D274" t="n">
-        <v>1</v>
+        <v>1.0001</v>
       </c>
       <c r="F274" t="n">
         <v>0</v>
@@ -4800,13 +4800,13 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.08108</v>
+        <v>0.08017000000000001</v>
       </c>
       <c r="D275" t="n">
-        <v>0.08097</v>
+        <v>0.08008</v>
       </c>
       <c r="F275" t="n">
-        <v>-0.14</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="276">
@@ -4816,13 +4816,13 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.009390000000000001</v>
+        <v>0.009339999999999999</v>
       </c>
       <c r="D276" t="n">
-        <v>0.00942</v>
+        <v>0.009350000000000001</v>
       </c>
       <c r="F276" t="n">
-        <v>0.32</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="277">
@@ -4832,10 +4832,10 @@
         </is>
       </c>
       <c r="B277" t="n">
-        <v>293</v>
+        <v>290.6</v>
       </c>
       <c r="D277" t="n">
-        <v>293</v>
+        <v>290.6</v>
       </c>
       <c r="F277" t="n">
         <v>0</v>
@@ -4848,13 +4848,13 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>0.15</v>
+        <v>0.1481</v>
       </c>
       <c r="D278" t="n">
-        <v>0.1496</v>
+        <v>0.1481</v>
       </c>
       <c r="F278" t="n">
-        <v>-0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -4864,13 +4864,13 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>0.703</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="D279" t="n">
-        <v>0.702</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F279" t="n">
-        <v>-0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280">
@@ -4880,10 +4880,10 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.585</v>
+        <v>0.586</v>
       </c>
       <c r="D280" t="n">
-        <v>0.585</v>
+        <v>0.586</v>
       </c>
       <c r="F280" t="n">
         <v>0</v>
@@ -4896,10 +4896,10 @@
         </is>
       </c>
       <c r="B281" t="n">
-        <v>0.1609</v>
+        <v>0.1593</v>
       </c>
       <c r="D281" t="n">
-        <v>0.1609</v>
+        <v>0.1593</v>
       </c>
       <c r="F281" t="n">
         <v>0</v>
@@ -4912,10 +4912,10 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>0.03483</v>
+        <v>0.03459</v>
       </c>
       <c r="D282" t="n">
-        <v>0.03482</v>
+        <v>0.03458</v>
       </c>
       <c r="F282" t="n">
         <v>-0.03</v>
@@ -4931,10 +4931,10 @@
         <v>1.279</v>
       </c>
       <c r="D283" t="n">
-        <v>1.277</v>
+        <v>1.279</v>
       </c>
       <c r="F283" t="n">
-        <v>-0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284">
@@ -4944,13 +4944,13 @@
         </is>
       </c>
       <c r="B284" t="n">
-        <v>0.532</v>
+        <v>0.528</v>
       </c>
       <c r="D284" t="n">
-        <v>0.531</v>
+        <v>0.528</v>
       </c>
       <c r="F284" t="n">
-        <v>-0.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285">
@@ -4960,13 +4960,13 @@
         </is>
       </c>
       <c r="B285" t="n">
-        <v>0.001293</v>
+        <v>0.001277</v>
       </c>
       <c r="D285" t="n">
-        <v>0.001292</v>
+        <v>0.00128</v>
       </c>
       <c r="F285" t="n">
-        <v>-0.08</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="286">
@@ -4976,13 +4976,13 @@
         </is>
       </c>
       <c r="B286" t="n">
-        <v>0.601</v>
+        <v>0.594</v>
       </c>
       <c r="D286" t="n">
-        <v>0.599</v>
+        <v>0.594</v>
       </c>
       <c r="F286" t="n">
-        <v>-0.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287">
@@ -4992,13 +4992,13 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>3.157</v>
+        <v>3.38</v>
       </c>
       <c r="D287" t="n">
-        <v>3.079</v>
+        <v>3.364</v>
       </c>
       <c r="F287" t="n">
-        <v>-2.47</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="288">
@@ -5008,13 +5008,13 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>0.4879</v>
+        <v>0.4889</v>
       </c>
       <c r="D288" t="n">
-        <v>0.4905</v>
+        <v>0.4889</v>
       </c>
       <c r="F288" t="n">
-        <v>0.53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289">
@@ -5024,13 +5024,13 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>0.04638</v>
+        <v>0.04609</v>
       </c>
       <c r="D289" t="n">
-        <v>0.04645</v>
+        <v>0.04609</v>
       </c>
       <c r="F289" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290">
@@ -5040,13 +5040,13 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>0.14874</v>
+        <v>0.145</v>
       </c>
       <c r="D290" t="n">
-        <v>0.14878</v>
+        <v>0.14486</v>
       </c>
       <c r="F290" t="n">
-        <v>0.03</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="291">
@@ -5056,13 +5056,13 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>0.293</v>
+        <v>0.287</v>
       </c>
       <c r="D291" t="n">
-        <v>0.294</v>
+        <v>0.287</v>
       </c>
       <c r="F291" t="n">
-        <v>0.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292">
@@ -5072,13 +5072,13 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>0.004332</v>
+        <v>0.00431</v>
       </c>
       <c r="D292" t="n">
-        <v>0.004331</v>
+        <v>0.004305</v>
       </c>
       <c r="F292" t="n">
-        <v>-0.02</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="293">
@@ -5088,13 +5088,13 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>0.354</v>
+        <v>0.348</v>
       </c>
       <c r="D293" t="n">
-        <v>0.357</v>
+        <v>0.348</v>
       </c>
       <c r="F293" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294">
@@ -5104,10 +5104,10 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>1.937</v>
+        <v>1.914</v>
       </c>
       <c r="D294" t="n">
-        <v>1.937</v>
+        <v>1.914</v>
       </c>
       <c r="F294" t="n">
         <v>0</v>
@@ -5120,13 +5120,13 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>1.414</v>
+        <v>1.394</v>
       </c>
       <c r="D295" t="n">
-        <v>1.401</v>
+        <v>1.394</v>
       </c>
       <c r="F295" t="n">
-        <v>-0.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296">
@@ -5136,13 +5136,13 @@
         </is>
       </c>
       <c r="B296" t="n">
-        <v>0.47384</v>
+        <v>0.46997</v>
       </c>
       <c r="D296" t="n">
-        <v>0.47499</v>
+        <v>0.46997</v>
       </c>
       <c r="F296" t="n">
-        <v>0.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297">
@@ -5152,13 +5152,13 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>117.8</v>
+        <v>117.6</v>
       </c>
       <c r="D297" t="n">
-        <v>118</v>
+        <v>117.6</v>
       </c>
       <c r="F297" t="n">
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298">
@@ -5184,13 +5184,13 @@
         </is>
       </c>
       <c r="B299" t="n">
-        <v>2.5506</v>
+        <v>2.5628</v>
       </c>
       <c r="D299" t="n">
-        <v>2.549</v>
+        <v>2.5671</v>
       </c>
       <c r="F299" t="n">
-        <v>-0.06</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="300">
@@ -5216,10 +5216,10 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>24.3</v>
+        <v>24</v>
       </c>
       <c r="D301" t="n">
-        <v>24.3</v>
+        <v>24</v>
       </c>
       <c r="F301" t="n">
         <v>0</v>
@@ -5232,10 +5232,10 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>5.9</v>
+        <v>5.92</v>
       </c>
       <c r="D302" t="n">
-        <v>5.9</v>
+        <v>5.92</v>
       </c>
       <c r="F302" t="n">
         <v>0</v>
@@ -5248,10 +5248,10 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>12.42</v>
+        <v>12.29</v>
       </c>
       <c r="D303" t="n">
-        <v>12.42</v>
+        <v>12.29</v>
       </c>
       <c r="F303" t="n">
         <v>0</v>
@@ -5264,10 +5264,10 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>0.03837</v>
+        <v>0.03821</v>
       </c>
       <c r="D304" t="n">
-        <v>0.03837</v>
+        <v>0.03821</v>
       </c>
       <c r="F304" t="n">
         <v>0</v>
@@ -5280,13 +5280,13 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>0.0156</v>
+        <v>0.0155</v>
       </c>
       <c r="D305" t="n">
         <v>0.0155</v>
       </c>
       <c r="F305" t="n">
-        <v>-0.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306">
@@ -5296,13 +5296,13 @@
         </is>
       </c>
       <c r="B306" t="n">
-        <v>0.2694</v>
+        <v>0.2684</v>
       </c>
       <c r="D306" t="n">
-        <v>0.2671</v>
+        <v>0.2684</v>
       </c>
       <c r="F306" t="n">
-        <v>-0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307">
@@ -5312,13 +5312,13 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>0.01258</v>
+        <v>0.012386</v>
       </c>
       <c r="D307" t="n">
-        <v>0.012583</v>
+        <v>0.012372</v>
       </c>
       <c r="F307" t="n">
-        <v>0.02</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="308">
@@ -5328,10 +5328,10 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>0.01286</v>
+        <v>0.01281</v>
       </c>
       <c r="D308" t="n">
-        <v>0.01286</v>
+        <v>0.01281</v>
       </c>
       <c r="F308" t="n">
         <v>0</v>
@@ -5360,13 +5360,13 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>4.66</v>
+        <v>4.64</v>
       </c>
       <c r="D310" t="n">
-        <v>4.67</v>
+        <v>4.64</v>
       </c>
       <c r="F310" t="n">
-        <v>0.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311">
@@ -5376,10 +5376,10 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>0.882</v>
+        <v>0.866</v>
       </c>
       <c r="D311" t="n">
-        <v>0.882</v>
+        <v>0.866</v>
       </c>
       <c r="F311" t="n">
         <v>0</v>
@@ -5392,10 +5392,10 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>32.8</v>
+        <v>32.7</v>
       </c>
       <c r="D312" t="n">
-        <v>32.8</v>
+        <v>32.7</v>
       </c>
       <c r="F312" t="n">
         <v>0</v>
@@ -5408,10 +5408,10 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>1.1</v>
+        <v>1.09</v>
       </c>
       <c r="D313" t="n">
-        <v>1.1</v>
+        <v>1.09</v>
       </c>
       <c r="F313" t="n">
         <v>0</v>
@@ -5424,10 +5424,10 @@
         </is>
       </c>
       <c r="B314" t="n">
-        <v>0.7564</v>
+        <v>0.7489</v>
       </c>
       <c r="D314" t="n">
-        <v>0.7564</v>
+        <v>0.7489</v>
       </c>
       <c r="F314" t="n">
         <v>0</v>
@@ -5456,13 +5456,13 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>0.659</v>
+        <v>0.652</v>
       </c>
       <c r="D316" t="n">
-        <v>0.658</v>
+        <v>0.652</v>
       </c>
       <c r="F316" t="n">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317">
@@ -5472,13 +5472,13 @@
         </is>
       </c>
       <c r="B317" t="n">
-        <v>0.739</v>
+        <v>0.736</v>
       </c>
       <c r="D317" t="n">
-        <v>0.741</v>
+        <v>0.736</v>
       </c>
       <c r="F317" t="n">
-        <v>0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318">
@@ -5488,10 +5488,10 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>0.125</v>
+        <v>0.1241</v>
       </c>
       <c r="D318" t="n">
-        <v>0.125</v>
+        <v>0.1241</v>
       </c>
       <c r="F318" t="n">
         <v>0</v>
@@ -5504,13 +5504,13 @@
         </is>
       </c>
       <c r="B319" t="n">
-        <v>0.6673</v>
+        <v>0.6612</v>
       </c>
       <c r="D319" t="n">
-        <v>0.6663</v>
+        <v>0.6612</v>
       </c>
       <c r="F319" t="n">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320">
@@ -5520,13 +5520,13 @@
         </is>
       </c>
       <c r="B320" t="n">
-        <v>0.00781</v>
+        <v>0.00773</v>
       </c>
       <c r="D320" t="n">
-        <v>0.0078</v>
+        <v>0.00773</v>
       </c>
       <c r="F320" t="n">
-        <v>-0.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321">
@@ -5536,10 +5536,10 @@
         </is>
       </c>
       <c r="B321" t="n">
-        <v>0.1304</v>
+        <v>0.1295</v>
       </c>
       <c r="D321" t="n">
-        <v>0.1304</v>
+        <v>0.1295</v>
       </c>
       <c r="F321" t="n">
         <v>0</v>
@@ -5568,13 +5568,13 @@
         </is>
       </c>
       <c r="B323" t="n">
-        <v>10.6</v>
+        <v>10.52</v>
       </c>
       <c r="D323" t="n">
-        <v>10.64</v>
+        <v>10.52</v>
       </c>
       <c r="F323" t="n">
-        <v>0.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324">
@@ -5584,13 +5584,13 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>0.0252</v>
+        <v>0.024</v>
       </c>
       <c r="D324" t="n">
-        <v>0.0251</v>
+        <v>0.0239</v>
       </c>
       <c r="F324" t="n">
-        <v>-0.4</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="325">
@@ -5600,10 +5600,10 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>0.0058</v>
+        <v>0.00574</v>
       </c>
       <c r="D325" t="n">
-        <v>0.0058</v>
+        <v>0.00574</v>
       </c>
       <c r="F325" t="n">
         <v>0</v>
@@ -5616,10 +5616,10 @@
         </is>
       </c>
       <c r="B326" t="n">
-        <v>0.03602</v>
+        <v>0.03565</v>
       </c>
       <c r="D326" t="n">
-        <v>0.03602</v>
+        <v>0.03565</v>
       </c>
       <c r="F326" t="n">
         <v>0</v>
@@ -5632,10 +5632,10 @@
         </is>
       </c>
       <c r="B327" t="n">
-        <v>0.2266</v>
+        <v>0.2237</v>
       </c>
       <c r="D327" t="n">
-        <v>0.2266</v>
+        <v>0.2237</v>
       </c>
       <c r="F327" t="n">
         <v>0</v>
@@ -5648,10 +5648,10 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>0.00138</v>
+        <v>0.00137</v>
       </c>
       <c r="D328" t="n">
-        <v>0.00138</v>
+        <v>0.00137</v>
       </c>
       <c r="F328" t="n">
         <v>0</v>
@@ -5664,13 +5664,13 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>0.0901</v>
+        <v>0.09394255</v>
       </c>
       <c r="D329" t="n">
-        <v>0.090105</v>
+        <v>0.09393517</v>
       </c>
       <c r="F329" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="330">
@@ -5680,10 +5680,10 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0.378</v>
+        <v>0.373</v>
       </c>
       <c r="D330" t="n">
-        <v>0.378</v>
+        <v>0.373</v>
       </c>
       <c r="F330" t="n">
         <v>0</v>
@@ -5696,10 +5696,10 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>0.1405</v>
+        <v>0.139</v>
       </c>
       <c r="D331" t="n">
-        <v>0.1405</v>
+        <v>0.139</v>
       </c>
       <c r="F331" t="n">
         <v>0</v>
@@ -5712,13 +5712,13 @@
         </is>
       </c>
       <c r="B332" t="n">
-        <v>0.02192</v>
+        <v>0.02193</v>
       </c>
       <c r="D332" t="n">
-        <v>0.0221</v>
+        <v>0.02176</v>
       </c>
       <c r="F332" t="n">
-        <v>0.82</v>
+        <v>-0.78</v>
       </c>
     </row>
     <row r="333">
@@ -5728,10 +5728,10 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0.9389999999999999</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="D333" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="F333" t="n">
         <v>-0.11</v>
@@ -5744,13 +5744,13 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>1.3143</v>
+        <v>1.2924</v>
       </c>
       <c r="D334" t="n">
-        <v>1.312</v>
+        <v>1.2924</v>
       </c>
       <c r="F334" t="n">
-        <v>-0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335">
@@ -5760,10 +5760,10 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>3.422</v>
+        <v>3.38</v>
       </c>
       <c r="D335" t="n">
-        <v>3.422</v>
+        <v>3.38</v>
       </c>
       <c r="F335" t="n">
         <v>0</v>
@@ -5776,13 +5776,13 @@
         </is>
       </c>
       <c r="B336" t="n">
-        <v>1.2532</v>
+        <v>1.2275</v>
       </c>
       <c r="D336" t="n">
-        <v>1.2568</v>
+        <v>1.2276</v>
       </c>
       <c r="F336" t="n">
-        <v>0.29</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="337">
@@ -5792,10 +5792,10 @@
         </is>
       </c>
       <c r="B337" t="n">
-        <v>1.691</v>
+        <v>1.675</v>
       </c>
       <c r="D337" t="n">
-        <v>1.691</v>
+        <v>1.675</v>
       </c>
       <c r="F337" t="n">
         <v>0</v>
@@ -5808,10 +5808,10 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>0.401</v>
+        <v>0.397</v>
       </c>
       <c r="D338" t="n">
-        <v>0.401</v>
+        <v>0.397</v>
       </c>
       <c r="F338" t="n">
         <v>0</v>
@@ -5824,13 +5824,13 @@
         </is>
       </c>
       <c r="B339" t="n">
-        <v>0.34487</v>
+        <v>0.31151</v>
       </c>
       <c r="D339" t="n">
-        <v>0.3421</v>
+        <v>0.31145</v>
       </c>
       <c r="F339" t="n">
-        <v>-0.8</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="340">
@@ -5840,13 +5840,13 @@
         </is>
       </c>
       <c r="B340" t="n">
-        <v>1.104</v>
+        <v>1.084</v>
       </c>
       <c r="D340" t="n">
-        <v>1.106</v>
+        <v>1.084</v>
       </c>
       <c r="F340" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341">
@@ -5856,10 +5856,10 @@
         </is>
       </c>
       <c r="B341" t="n">
-        <v>0.1883</v>
+        <v>0.1844</v>
       </c>
       <c r="D341" t="n">
-        <v>0.1883</v>
+        <v>0.1844</v>
       </c>
       <c r="F341" t="n">
         <v>0</v>
@@ -5888,10 +5888,10 @@
         </is>
       </c>
       <c r="B343" t="n">
-        <v>0.0472</v>
+        <v>0.0471</v>
       </c>
       <c r="D343" t="n">
-        <v>0.0472</v>
+        <v>0.0471</v>
       </c>
       <c r="F343" t="n">
         <v>0</v>
@@ -5904,13 +5904,13 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>0.0675</v>
+        <v>0.066</v>
       </c>
       <c r="D344" t="n">
-        <v>0.0678</v>
+        <v>0.0659</v>
       </c>
       <c r="F344" t="n">
-        <v>0.44</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="345">
@@ -5920,13 +5920,13 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>1.39297</v>
+        <v>1.37532</v>
       </c>
       <c r="D345" t="n">
-        <v>1.3921</v>
+        <v>1.37515</v>
       </c>
       <c r="F345" t="n">
-        <v>-0.06</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="346">
@@ -5936,13 +5936,13 @@
         </is>
       </c>
       <c r="B346" t="n">
-        <v>2.26</v>
+        <v>2.259</v>
       </c>
       <c r="D346" t="n">
-        <v>2.266</v>
+        <v>2.259</v>
       </c>
       <c r="F346" t="n">
-        <v>0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347">
@@ -5952,13 +5952,13 @@
         </is>
       </c>
       <c r="B347" t="n">
-        <v>7.4</v>
+        <v>7.335</v>
       </c>
       <c r="D347" t="n">
-        <v>7.397</v>
+        <v>7.3311</v>
       </c>
       <c r="F347" t="n">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="348">
@@ -5968,13 +5968,13 @@
         </is>
       </c>
       <c r="B348" t="n">
-        <v>3.515</v>
+        <v>3.4979</v>
       </c>
       <c r="D348" t="n">
-        <v>3.5149</v>
+        <v>3.4979</v>
       </c>
       <c r="F348" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349">
@@ -5984,10 +5984,10 @@
         </is>
       </c>
       <c r="B349" t="n">
-        <v>0.6212</v>
+        <v>0.6194</v>
       </c>
       <c r="D349" t="n">
-        <v>0.6212</v>
+        <v>0.6194</v>
       </c>
       <c r="F349" t="n">
         <v>0</v>
@@ -6000,13 +6000,13 @@
         </is>
       </c>
       <c r="B350" t="n">
-        <v>4.665</v>
+        <v>4.67</v>
       </c>
       <c r="D350" t="n">
-        <v>4.682</v>
+        <v>4.704</v>
       </c>
       <c r="F350" t="n">
-        <v>0.36</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="351">
@@ -6016,10 +6016,10 @@
         </is>
       </c>
       <c r="B351" t="n">
-        <v>5.37</v>
+        <v>5.34</v>
       </c>
       <c r="D351" t="n">
-        <v>5.37</v>
+        <v>5.34</v>
       </c>
       <c r="F351" t="n">
         <v>0</v>
@@ -6032,13 +6032,13 @@
         </is>
       </c>
       <c r="B352" t="n">
-        <v>2.4004</v>
+        <v>2.512</v>
       </c>
       <c r="D352" t="n">
-        <v>2.4063</v>
+        <v>2.5299</v>
       </c>
       <c r="F352" t="n">
-        <v>0.25</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="353">
@@ -6048,13 +6048,13 @@
         </is>
       </c>
       <c r="B353" t="n">
+        <v>1.13e-06</v>
+      </c>
+      <c r="D353" t="n">
         <v>1.14e-06</v>
       </c>
-      <c r="D353" t="n">
-        <v>1.13e-06</v>
-      </c>
       <c r="F353" t="n">
-        <v>-0.88</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="354">
@@ -6064,10 +6064,10 @@
         </is>
       </c>
       <c r="B354" t="n">
-        <v>0.005426</v>
+        <v>0.005414</v>
       </c>
       <c r="D354" t="n">
-        <v>0.005426</v>
+        <v>0.005414</v>
       </c>
       <c r="F354" t="n">
         <v>0</v>
@@ -6080,10 +6080,10 @@
         </is>
       </c>
       <c r="B355" t="n">
-        <v>1.968</v>
+        <v>1.946</v>
       </c>
       <c r="D355" t="n">
-        <v>1.968</v>
+        <v>1.946</v>
       </c>
       <c r="F355" t="n">
         <v>0</v>
@@ -6096,10 +6096,10 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>1.965</v>
+        <v>1.946</v>
       </c>
       <c r="D356" t="n">
-        <v>1.965</v>
+        <v>1.946</v>
       </c>
       <c r="F356" t="n">
         <v>0</v>
@@ -6112,10 +6112,10 @@
         </is>
       </c>
       <c r="B357" t="n">
-        <v>1.289</v>
+        <v>1.283</v>
       </c>
       <c r="D357" t="n">
-        <v>1.289</v>
+        <v>1.283</v>
       </c>
       <c r="F357" t="n">
         <v>0</v>
@@ -6128,13 +6128,13 @@
         </is>
       </c>
       <c r="B358" t="n">
-        <v>5.704</v>
+        <v>5.674</v>
       </c>
       <c r="D358" t="n">
-        <v>5.701</v>
+        <v>5.674</v>
       </c>
       <c r="F358" t="n">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -6144,10 +6144,10 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>1.092</v>
+        <v>1.088</v>
       </c>
       <c r="D359" t="n">
-        <v>1.092</v>
+        <v>1.088</v>
       </c>
       <c r="F359" t="n">
         <v>0</v>
@@ -6160,10 +6160,10 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>0.001999</v>
+        <v>0.001941</v>
       </c>
       <c r="D360" t="n">
-        <v>0.001998</v>
+        <v>0.00194</v>
       </c>
       <c r="F360" t="n">
         <v>-0.05</v>

</xml_diff>